<commit_message>
matrices 2a and 2b
</commit_message>
<xml_diff>
--- a/hw10/10_2.xlsx
+++ b/hw10/10_2.xlsx
@@ -107,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +395,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +515,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2">
@@ -559,48 +560,20 @@
       <c r="R2" t="s">
         <v>0</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -609,7 +582,7 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3">
@@ -651,48 +624,20 @@
       <c r="R3" t="s">
         <v>1</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -704,7 +649,7 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1">
@@ -743,48 +688,20 @@
       <c r="R4" t="s">
         <v>2</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>1</v>
-      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -799,13 +716,13 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5">
@@ -835,48 +752,20 @@
       <c r="R5" t="s">
         <v>3</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -894,7 +783,7 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
@@ -927,48 +816,20 @@
       <c r="R6" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -989,7 +850,7 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7">
@@ -1019,48 +880,20 @@
       <c r="R7" t="s">
         <v>5</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1084,7 +917,7 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>1</v>
       </c>
       <c r="I8">
@@ -1111,48 +944,20 @@
       <c r="R8" t="s">
         <v>6</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1179,7 +984,7 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>1</v>
       </c>
       <c r="J9">
@@ -1203,48 +1008,20 @@
       <c r="R9" t="s">
         <v>7</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1274,7 +1051,7 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10">
@@ -1295,48 +1072,20 @@
       <c r="R10" t="s">
         <v>8</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1369,7 +1118,7 @@
       <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>1</v>
       </c>
       <c r="L11">
@@ -1387,48 +1136,20 @@
       <c r="R11" t="s">
         <v>9</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1464,7 +1185,7 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>1</v>
       </c>
       <c r="M12">
@@ -1479,48 +1200,20 @@
       <c r="R12" t="s">
         <v>10</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" s="1">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1559,7 +1252,7 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1">
         <v>1</v>
       </c>
       <c r="N13" s="1">
@@ -1571,48 +1264,20 @@
       <c r="R13" t="s">
         <v>11</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1654,7 +1319,7 @@
       <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>1</v>
       </c>
       <c r="O14">
@@ -1663,48 +1328,20 @@
       <c r="R14" t="s">
         <v>12</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
-      </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1749,54 +1386,26 @@
       <c r="N15">
         <v>0</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <v>1</v>
       </c>
       <c r="R15" t="s">
         <v>13</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15" s="1">
-        <v>1</v>
-      </c>
-      <c r="V15" s="1">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>